<commit_message>
Added totals to product backlog
</commit_message>
<xml_diff>
--- a/admin/product_backlog.xlsx
+++ b/admin/product_backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Work Items</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Implementation of basics</t>
+  </si>
+  <si>
+    <t>Total:</t>
   </si>
 </sst>
 </file>
@@ -522,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -782,6 +785,31 @@
         <v>14.4</v>
       </c>
     </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2">
+        <f>SUM(B2:B12)</f>
+        <v>49.5</v>
+      </c>
+      <c r="C13" s="2">
+        <f>SUM(C2:C12)</f>
+        <v>2.15</v>
+      </c>
+      <c r="D13" s="2">
+        <f>SUM(D2:D12)</f>
+        <v>59.55</v>
+      </c>
+      <c r="E13" s="2">
+        <f>SUM(E2:E12)</f>
+        <v>59.55</v>
+      </c>
+      <c r="F13" s="2">
+        <f>SUM(F2:F12)</f>
+        <v>51.65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
updated product backlog to current status
</commit_message>
<xml_diff>
--- a/admin/product_backlog.xlsx
+++ b/admin/product_backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="14400" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Work Items</t>
   </si>
@@ -67,6 +67,21 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>Implementation of MarketPlace</t>
+  </si>
+  <si>
+    <t>Implementing planets and Universe</t>
+  </si>
+  <si>
+    <t>Implementing ShipYard</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>UI Evaluation</t>
   </si>
 </sst>
 </file>
@@ -123,8 +138,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -165,7 +186,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -181,6 +202,9 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -196,6 +220,9 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -525,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -785,29 +812,129 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:7" ht="30">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1">
+        <v>11</v>
+      </c>
+      <c r="F14" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="1">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E16" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="F16" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="1">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="D17" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="E17" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2">
-        <f>SUM(B2:B12)</f>
-        <v>49.5</v>
-      </c>
-      <c r="C13" s="2">
-        <f>SUM(C2:C12)</f>
-        <v>2.15</v>
-      </c>
-      <c r="D13" s="2">
-        <f>SUM(D2:D12)</f>
-        <v>59.55</v>
-      </c>
-      <c r="E13" s="2">
-        <f>SUM(E2:E12)</f>
-        <v>59.55</v>
-      </c>
-      <c r="F13" s="2">
-        <f>SUM(F2:F12)</f>
-        <v>51.65</v>
+      <c r="B20" s="2">
+        <f>SUM(B2:B17)</f>
+        <v>84.5</v>
+      </c>
+      <c r="C20" s="2">
+        <f>SUM(C2:C17)</f>
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="D20" s="2">
+        <f>SUM(D2:D17)</f>
+        <v>96.55</v>
+      </c>
+      <c r="E20" s="2">
+        <f>SUM(E2:E17)</f>
+        <v>96.55</v>
+      </c>
+      <c r="F20" s="2">
+        <f>SUM(F1:F17)</f>
+        <v>78.650000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated last minute demo changes
</commit_message>
<xml_diff>
--- a/admin/product_backlog.xlsx
+++ b/admin/product_backlog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-20" windowWidth="14400" windowHeight="17460" tabRatio="500"/>
@@ -555,7 +555,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -588,9 +588,7 @@
       <c r="F1" s="2">
         <v>2</v>
       </c>
-      <c r="G1" s="2">
-        <v>3</v>
-      </c>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">

</xml_diff>